<commit_message>
pdf rows & columns working
</commit_message>
<xml_diff>
--- a/nerdle_output_turkheimer.xlsx
+++ b/nerdle_output_turkheimer.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,7 +555,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>mean</t>
+          <t>mean score</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -647,46 +647,184 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>group total played</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3890</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4378</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3868</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3958</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3889</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3974</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3952</v>
+      </c>
+      <c r="I5" t="n">
+        <v>4001</v>
+      </c>
+      <c r="J5" t="n">
+        <v>4159</v>
+      </c>
+      <c r="K5" t="n">
+        <v>4318</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4063</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4237</v>
+      </c>
+      <c r="N5" t="n">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>group mean</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.1159</v>
+      </c>
+      <c r="C6" t="n">
+        <v>4.1039</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.1107</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.0942</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4.1273</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4.079</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.1015</v>
+      </c>
+      <c r="I6" t="n">
+        <v>4.1135</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4.076</v>
+      </c>
+      <c r="K6" t="n">
+        <v>4.1061</v>
+      </c>
+      <c r="L6" t="n">
+        <v>4.1088</v>
+      </c>
+      <c r="M6" t="n">
+        <v>4.0991</v>
+      </c>
+      <c r="N6" t="n">
+        <v>4.1024</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>group st. dev.</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.0605</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.056</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.0586</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.0519</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.0613</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1.0461</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.0554</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1.0603</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1.0512</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.0569</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1.0599</v>
+      </c>
+      <c r="M7" t="n">
+        <v>1.0591</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.0562</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>p-value</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B8" t="n">
         <v>0.1075</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C8" t="n">
         <v>0.9999</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D8" t="n">
         <v>0.929</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E8" t="n">
         <v>0.4886</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F8" t="n">
         <v>0.0036</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G8" t="n">
         <v>0.0162</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H8" t="n">
         <v>0.9978</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I8" t="n">
         <v>0.486</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J8" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K8" t="n">
         <v>0.4353</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L8" t="n">
         <v>0.5646</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M8" t="n">
         <v>0.66</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N8" t="n">
         <v>0.1893</v>
       </c>
     </row>

</xml_diff>